<commit_message>
reversing order of posts on home page
</commit_message>
<xml_diff>
--- a/assets/xls/2022_ColoradoSprings.xlsx
+++ b/assets/xls/2022_ColoradoSprings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F66DC8-4D58-4FD7-A8B8-DD9B9EF813DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FB04DAA-D65E-470F-BD73-6A7DC7203198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="435" windowWidth="24675" windowHeight="15315" xr2:uid="{6FE3E817-6BA9-4291-A0BA-63087DBF9607}"/>
+    <workbookView xWindow="30930" yWindow="270" windowWidth="24675" windowHeight="15315" xr2:uid="{6FE3E817-6BA9-4291-A0BA-63087DBF9607}"/>
   </bookViews>
   <sheets>
     <sheet name="New Event Checklist" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>New SQL Saturday Event</t>
   </si>
@@ -126,12 +126,6 @@
     <t>SQL Saturday Colorado Springs 2022</t>
   </si>
   <si>
-    <t>Mar 21, 2022</t>
-  </si>
-  <si>
-    <t>1000 - 1630 MST</t>
-  </si>
-  <si>
     <t>Library 21c 1175 Chapel Hills Dr, Colorado Springs, CO 80920</t>
   </si>
   <si>
@@ -139,6 +133,18 @@
   </si>
   <si>
     <t>Springs SQL</t>
+  </si>
+  <si>
+    <t>Mar 19, 2022</t>
+  </si>
+  <si>
+    <t>1000 - 1730 MST</t>
+  </si>
+  <si>
+    <t>https://www.eventbrite.com/e/sql-saturday-colorado-springs-tickets-247770376867</t>
+  </si>
+  <si>
+    <t>springssql@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -578,13 +584,13 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="146.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="51.85546875" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" customWidth="1"/>
@@ -649,12 +655,12 @@
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="6" t="str">
         <f>+C7</f>
-        <v>Mar 21, 2022</v>
+        <v>Mar 19, 2022</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -669,12 +675,12 @@
         <v>26</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="6" t="str">
         <f>+C8</f>
-        <v>1000 - 1630 MST</v>
+        <v>1000 - 1730 MST</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>27</v>
@@ -717,15 +723,17 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>X</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="E11" s="10">
+      <c r="C11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://www.eventbrite.com/e/sql-saturday-colorado-springs-tickets-247770376867</v>
       </c>
       <c r="F11" s="7"/>
     </row>
@@ -738,7 +746,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" s="10" t="str">
         <f t="shared" si="1"/>
@@ -757,7 +765,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E13" s="10" t="str">
         <f t="shared" si="1"/>
@@ -776,7 +784,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="10" t="str">
         <f t="shared" si="1"/>
@@ -789,15 +797,17 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> </v>
+        <v>X</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="E15" s="10">
+      <c r="C15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>springssql@gmail.com</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>21</v>
@@ -925,8 +935,10 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F15" r:id="rId1" xr:uid="{A1038F06-E7F0-41F5-8670-A25ADE817599}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{847FACCD-90BB-4313-8F18-61B6C1B495B4}"/>
+    <hyperlink ref="C15" r:id="rId3" xr:uid="{8FEA9729-4947-45E5-85B7-6880AEF1823E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>